<commit_message>
Add jumpers + note
Add jumpers to schematic, drawing and BOM.
Add note about removal of Kapton from DIP switches to drawing.
</commit_message>
<xml_diff>
--- a/Source/Project Outputs for RUMBA_plus/RUMBA_plus_BOM_1_4_2A.xlsx
+++ b/Source/Project Outputs for RUMBA_plus/RUMBA_plus_BOM_1_4_2A.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DD1CBA8-6D82-4F6B-AB73-B437881CF636}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BD384B1-8794-4C8F-B0DA-57D281524ACC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="1035" windowWidth="4110" windowHeight="10725" xr2:uid="{6E3CBB45-E391-45B8-9977-20EBF38CA5F1}"/>
+    <workbookView xWindow="1035" yWindow="1035" windowWidth="4110" windowHeight="10725" xr2:uid="{ED978A29-247A-4233-81ED-B0EF55EC4E6A}"/>
   </bookViews>
   <sheets>
     <sheet name="RUMBA_plus_BOM_1_4_2A" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="218">
   <si>
     <t>Designator</t>
   </si>
@@ -52,6 +52,27 @@
     <t>Supplier Part Number 1</t>
   </si>
   <si>
+    <t>JMP</t>
+  </si>
+  <si>
+    <t>2.54mm .1" PCB Jumper, Green</t>
+  </si>
+  <si>
+    <t>Installed as per drawing, approved sub OK</t>
+  </si>
+  <si>
+    <t>Sullins</t>
+  </si>
+  <si>
+    <t>QPC02SXGN-RC</t>
+  </si>
+  <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>S9337-ND</t>
+  </si>
+  <si>
     <t>C1, C21, C22, C23, C24, C25, C30, C31, C32</t>
   </si>
   <si>
@@ -65,9 +86,6 @@
   </si>
   <si>
     <t>EEEFT1V101AP</t>
-  </si>
-  <si>
-    <t>Digi-Key</t>
   </si>
   <si>
     <t>PCE5016CT-ND</t>
@@ -1055,8 +1073,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A739788-9404-4467-84E4-87443BA2DD30}">
-  <dimension ref="A1:H49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E7E2C8-73B6-45E8-B6DD-185367C2FFCC}">
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1064,12 +1082,12 @@
   <cols>
     <col min="1" max="1" width="35.28515625" customWidth="1"/>
     <col min="2" max="2" width="37.140625" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="38.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1106,7 +1124,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="3">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
@@ -1132,1368 +1150,1397 @@
         <v>16</v>
       </c>
       <c r="C3" s="3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C9" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C10" s="3">
         <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C11" s="3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C12" s="3">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C13" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C17" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C18" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>92</v>
+        <v>13</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C19" s="3">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C20" s="3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="3">
-        <v>10</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>91</v>
-      </c>
       <c r="F21" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C22" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C23" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C24" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C25" s="3">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C26" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C27" s="3">
         <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C28" s="3">
         <v>1</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C29" s="3">
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C30" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C31" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C32" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C33" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C34" s="3">
         <v>1</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C35" s="3">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>17</v>
+        <v>152</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C36" s="3">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C37" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C38" s="3">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>163</v>
+        <v>23</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C39" s="3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>17</v>
+        <v>169</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C40" s="3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C41" s="3">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C42" s="3">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C43" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>184</v>
+        <v>23</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C44" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C45" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C46" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C47" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C48" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C49" s="3">
+        <v>6</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C50" s="3">
         <v>1</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H49" s="4" t="s">
-        <v>211</v>
+      <c r="D50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" tooltip="Component" display="'Panasonic" xr:uid="{0C0329C5-9F73-4DDF-BC35-68FBCBBC2681}"/>
-    <hyperlink ref="F2" r:id="rId2" tooltip="Manufacturer" display="'EEEFT1V101AP" xr:uid="{37078D43-0DCC-483E-A003-FD50A340EA25}"/>
-    <hyperlink ref="H2" r:id="rId3" tooltip="Supplier" display="'PCE5016CT-ND" xr:uid="{5E0D7D5E-0AFE-4D8E-AE3F-C14354EEE06F}"/>
-    <hyperlink ref="E3" r:id="rId4" tooltip="Component" display="'Yageo" xr:uid="{1056DB93-0D5C-45E8-BF22-FDA6CABBB128}"/>
-    <hyperlink ref="F3" r:id="rId5" tooltip="Manufacturer" display="'CC0603KRX7R9BB104" xr:uid="{51F9984F-2FFC-4A97-8E5F-EF476B794B59}"/>
-    <hyperlink ref="H3" r:id="rId6" tooltip="Supplier" display="'311-1344-1-ND" xr:uid="{2986A1C0-67FB-4FD8-9681-BC00B8BC6405}"/>
-    <hyperlink ref="E4" r:id="rId7" tooltip="Component" display="'Taiyo Yuden" xr:uid="{5E5A34C9-FBE2-401A-9F3A-83A6F80CFF39}"/>
-    <hyperlink ref="F4" r:id="rId8" tooltip="Manufacturer" display="'EMK107B7105KA-T" xr:uid="{EE749BC6-E27F-4FC3-A275-376EE809DAB1}"/>
-    <hyperlink ref="H4" r:id="rId9" tooltip="Supplier" display="'587-1241-1-ND" xr:uid="{5BE660DA-303A-4DA3-8927-C35A668EE807}"/>
-    <hyperlink ref="E5" r:id="rId10" tooltip="Component" display="'TDK" xr:uid="{5F1D51E0-B457-4502-9839-B6F70CD906ED}"/>
-    <hyperlink ref="F5" r:id="rId11" tooltip="Manufacturer" display="'C2012X7R1A475K085AC" xr:uid="{D77D4D48-BBDB-431B-BB54-2FA3E17255FB}"/>
-    <hyperlink ref="H5" r:id="rId12" tooltip="Supplier" display="'445-14527-1-ND" xr:uid="{03740853-CA7B-449A-BCEE-7C5F564BCEE4}"/>
-    <hyperlink ref="E6" r:id="rId13" tooltip="Component" display="'KEMET" xr:uid="{7930DF64-0FEA-4295-8669-814369D63A7E}"/>
-    <hyperlink ref="F6" r:id="rId14" tooltip="Manufacturer" display="'C1210C475K5RACTU" xr:uid="{CC8F8909-2ACF-462C-8EEF-C8DDF0DF8AA4}"/>
-    <hyperlink ref="H6" r:id="rId15" tooltip="Supplier" display="'399-6785-1-ND" xr:uid="{ECE218BD-5F35-4B02-9F56-FC028C981690}"/>
-    <hyperlink ref="E7" r:id="rId16" tooltip="Component" display="'Kyocera AVX" xr:uid="{CA85B60B-859D-482B-80CD-85E762387697}"/>
-    <hyperlink ref="F7" r:id="rId17" tooltip="Manufacturer" display="'06035C220JAT2A" xr:uid="{D7F739B6-52D9-4F08-BEDA-37CE7ACA8DBC}"/>
-    <hyperlink ref="H7" r:id="rId18" tooltip="Supplier" display="'478-6204-1-ND" xr:uid="{A2A6B740-8054-4C5A-A470-B944A0916314}"/>
-    <hyperlink ref="E8" r:id="rId19" tooltip="Component" display="'Molex" xr:uid="{AAA41D62-E9D1-4DC3-8951-7C4FE9EFC323}"/>
-    <hyperlink ref="F8" r:id="rId20" tooltip="Manufacturer" display="'105017-0001" xr:uid="{3EFEBFAF-6F22-48BF-8B13-D58DD1B5C35C}"/>
-    <hyperlink ref="H8" r:id="rId21" tooltip="Supplier" display="'WM1399CT-ND" xr:uid="{94BEA9AE-BA55-4915-A780-C913447D4C03}"/>
-    <hyperlink ref="E9" r:id="rId22" tooltip="Component" display="'Epson" xr:uid="{E276018B-CF36-4C82-89FD-06B994A5FF84}"/>
-    <hyperlink ref="F9" r:id="rId23" tooltip="Manufacturer" display="'FA-23816.0000MBC3" xr:uid="{28738642-C4B7-46E1-8CD1-1D457007BE82}"/>
-    <hyperlink ref="H9" r:id="rId24" tooltip="Supplier" display="'SER3686CT-ND" xr:uid="{C33B0104-C8C5-45D2-A5BE-159B6C2C7C36}"/>
-    <hyperlink ref="E10" r:id="rId25" tooltip="Component" display="'MCC" xr:uid="{192367D9-D0A3-401C-8E1E-A90E516C3C5F}"/>
-    <hyperlink ref="F10" r:id="rId26" tooltip="Manufacturer" display="'1N4148WX-TP" xr:uid="{B8FA415B-BC14-4A49-8E15-D406B76B0454}"/>
-    <hyperlink ref="H10" r:id="rId27" tooltip="Supplier" display="'1N4148WXTPMSCT-ND" xr:uid="{7CE01AC9-5955-4151-922B-0E693DDB818D}"/>
-    <hyperlink ref="E11" r:id="rId28" tooltip="Component" display="'Diodes" xr:uid="{783F6870-15EA-49CB-BACA-43A56BF0279D}"/>
-    <hyperlink ref="F11" r:id="rId29" tooltip="Manufacturer" display="'S2BA-13-F" xr:uid="{807B9E95-16EB-4746-9887-46688A159C0E}"/>
-    <hyperlink ref="H11" r:id="rId30" tooltip="Supplier" display="'S2BA-FDICT-ND" xr:uid="{0223ECD2-D0C4-4679-8C36-FAB375E1666A}"/>
-    <hyperlink ref="E12" r:id="rId31" tooltip="Component" display="'ON Semiconductor / Fairchild" xr:uid="{D6F6463D-456D-4FB4-BA41-247C39C29FF8}"/>
-    <hyperlink ref="F12" r:id="rId32" tooltip="Manufacturer" display="'SS24FL" xr:uid="{BBABC959-A183-4234-BC73-7C3AB842BDCB}"/>
-    <hyperlink ref="H12" r:id="rId33" tooltip="Supplier" display="'SS24FLCT-ND" xr:uid="{66F9D250-6F9E-4AC5-A972-29EEEA65F50D}"/>
-    <hyperlink ref="E13" r:id="rId34" tooltip="Component" display="'General Instruments" xr:uid="{1FEC9ACE-80B7-4F5D-96D0-18C9E20D03A4}"/>
-    <hyperlink ref="F13" r:id="rId35" tooltip="Manufacturer" display="'SSB44-E3/52T" xr:uid="{75B8F4DC-A55E-42E1-92BE-EF66C2CD70C7}"/>
-    <hyperlink ref="H13" r:id="rId36" tooltip="Supplier" display="'SSB44-E3/52TGICT-ND" xr:uid="{28E5DC28-D4F1-40E7-8FA0-569229D3C2F8}"/>
-    <hyperlink ref="E14" r:id="rId37" tooltip="Component" display="'Murata" xr:uid="{6F23F6FF-4FE0-402D-8695-3B589241FBA0}"/>
-    <hyperlink ref="F14" r:id="rId38" tooltip="Manufacturer" display="'BLM21PG221SN1D" xr:uid="{37566334-B6AA-40B2-B18D-8A9A7A40E355}"/>
-    <hyperlink ref="H14" r:id="rId39" tooltip="Supplier" display="'490-1054-1-ND" xr:uid="{1DA7C8F7-1E28-43C2-8B72-01301C69F732}"/>
-    <hyperlink ref="E15" r:id="rId40" tooltip="Component" display="'Bourns" xr:uid="{9E1379FF-64D0-4D3A-85E3-B7786396F59F}"/>
-    <hyperlink ref="F15" r:id="rId41" tooltip="Manufacturer" display="'SRN6045TA-4R7M" xr:uid="{13E3C4F0-C80B-4A64-9E51-CAA3FEB9C46F}"/>
-    <hyperlink ref="H15" r:id="rId42" tooltip="Supplier" display="'SRN6045TA-4R7MCT-ND" xr:uid="{92DAF81D-0CEC-4CFC-B77A-A2591F344ADF}"/>
-    <hyperlink ref="E16" r:id="rId43" tooltip="Component" display="'Bourns" xr:uid="{8B7F2369-EA28-474D-B921-17E4484A04BC}"/>
-    <hyperlink ref="F16" r:id="rId44" tooltip="Manufacturer" display="'SRN6045TA-330M" xr:uid="{6F44DAD3-3091-4EE5-85E4-45BC369A59A1}"/>
-    <hyperlink ref="H16" r:id="rId45" tooltip="Supplier" display="'SRN6045TA-330MCT-ND" xr:uid="{7D77A705-63F7-4CBF-8F31-C00BE4FB2325}"/>
-    <hyperlink ref="E17" r:id="rId46" tooltip="Component" display="'Memory Protection Devices" xr:uid="{6BBFE8D9-6A40-4CDA-AA79-BF98ED2A55FA}"/>
-    <hyperlink ref="F17" r:id="rId47" tooltip="Manufacturer" display="'BK-6013" xr:uid="{A9914245-C616-4BFD-98C9-AA64DD381519}"/>
-    <hyperlink ref="H17" r:id="rId48" tooltip="Supplier" display="'BK-6013-ND" xr:uid="{B98ECBFF-EE5A-4A66-A551-4C4BE184AD32}"/>
-    <hyperlink ref="E18" tooltip="Component" display="'Generic Header" xr:uid="{CC04CE66-0B0B-4957-BF0A-4BDBA7E18F2A}"/>
-    <hyperlink ref="F18" tooltip="Manufacturer" display="'" xr:uid="{F9EC4571-EBB7-4B4F-AF9A-BF9079B08830}"/>
-    <hyperlink ref="H18" tooltip="Supplier" display="'" xr:uid="{2F109A55-50C3-478C-9B74-BD101CA1F72C}"/>
-    <hyperlink ref="E19" tooltip="Component" display="'Generic Header" xr:uid="{1E96A785-F679-4A84-89C4-520437B4589A}"/>
-    <hyperlink ref="F19" tooltip="Manufacturer" display="'" xr:uid="{30732821-716D-4C6B-A154-48B2D88F9D3F}"/>
-    <hyperlink ref="H19" tooltip="Supplier" display="'" xr:uid="{F55F86AD-2C9D-40C3-8667-99E41FA48907}"/>
-    <hyperlink ref="E20" tooltip="Component" display="'Generic Header" xr:uid="{B46A1EE8-6211-441C-8B06-29CFE0F1E747}"/>
-    <hyperlink ref="F20" tooltip="Manufacturer" display="'" xr:uid="{22E6B238-2A15-41CE-B7E8-F48CEE46A294}"/>
-    <hyperlink ref="H20" tooltip="Supplier" display="'" xr:uid="{0DB33C10-E180-4A3A-9F08-15536873F8CF}"/>
-    <hyperlink ref="E21" tooltip="Component" display="'Generic Header" xr:uid="{32BB6F29-C8EB-422A-A018-268BB06D19C8}"/>
-    <hyperlink ref="F21" tooltip="Manufacturer" display="'" xr:uid="{101DC445-B18F-4F21-9B84-B538D649FD02}"/>
-    <hyperlink ref="H21" tooltip="Supplier" display="'" xr:uid="{D02E1B70-7CEF-44AB-B1B0-27CAB3DF18A7}"/>
-    <hyperlink ref="E22" tooltip="Component" display="'Generic Header" xr:uid="{76C8C7CB-8D62-4998-A614-B10C79126BC4}"/>
-    <hyperlink ref="F22" tooltip="Manufacturer" display="'" xr:uid="{D64F38EF-5F89-414F-A09C-68DD446726C5}"/>
-    <hyperlink ref="H22" tooltip="Supplier" display="'" xr:uid="{84E6D0B8-D155-4C91-9B7D-E128640440BF}"/>
-    <hyperlink ref="E23" tooltip="Component" display="'Generic Header" xr:uid="{B0682B55-45CC-40DC-84ED-7EDD1E2F9342}"/>
-    <hyperlink ref="F23" tooltip="Manufacturer" display="'" xr:uid="{1C1C65F4-021A-474A-981A-2319B4674830}"/>
-    <hyperlink ref="H23" tooltip="Supplier" display="'" xr:uid="{D70B34CF-6076-4C56-A5D0-D0A4E6ABA116}"/>
-    <hyperlink ref="E24" tooltip="Component" display="'Generic Header" xr:uid="{A2BCFD20-ADB9-4299-BBAB-43690D5DB3A1}"/>
-    <hyperlink ref="F24" tooltip="Manufacturer" display="'" xr:uid="{101F9E6D-6D6A-420A-8879-F31976E11079}"/>
-    <hyperlink ref="H24" tooltip="Supplier" display="'" xr:uid="{5793348E-CA35-4F63-B065-AE7AC6142374}"/>
-    <hyperlink ref="E25" tooltip="Component" display="'Generic Header" xr:uid="{F5261FB6-DC3E-4B06-B02A-C1F831CB4B39}"/>
-    <hyperlink ref="F25" tooltip="Manufacturer" display="'" xr:uid="{3F7412E2-EB88-438D-8798-018B74755C4F}"/>
-    <hyperlink ref="H25" tooltip="Supplier" display="'" xr:uid="{9FAF6A5E-647E-4E49-974A-28E605C815CB}"/>
-    <hyperlink ref="E26" r:id="rId49" tooltip="Component" display="'Microchip" xr:uid="{B3B8477F-AC1B-4B00-BC93-4CD2E96A253F}"/>
-    <hyperlink ref="F26" r:id="rId50" tooltip="Manufacturer" display="'ATMEGA16U2-MU" xr:uid="{55E0A7D5-B56D-46DC-BAE4-07849B11341C}"/>
-    <hyperlink ref="H26" r:id="rId51" tooltip="Supplier" display="'ATMEGA16U2-MU-ND" xr:uid="{C75071B3-CC07-481B-98DB-8323D583212E}"/>
-    <hyperlink ref="E27" r:id="rId52" tooltip="Component" display="'Microchip / Atmel" xr:uid="{A9DBB00F-A7BE-4FD3-8C82-7C03926F0A09}"/>
-    <hyperlink ref="F27" r:id="rId53" tooltip="Manufacturer" display="'ATMEGA2560-16AU" xr:uid="{E0B627E4-5D45-4273-9AD6-F21DA0C6D1EB}"/>
-    <hyperlink ref="H27" r:id="rId54" tooltip="Supplier" display="'ATMEGA2560-16AU-ND" xr:uid="{0B1F6F1A-93AE-44D4-8735-00C86635AA75}"/>
-    <hyperlink ref="E28" r:id="rId55" tooltip="Component" display="'Alpha &amp; Omega Semiconductor" xr:uid="{BD0EDDD4-47C7-4C34-8945-554BF3CFF58E}"/>
-    <hyperlink ref="F28" r:id="rId56" tooltip="Manufacturer" display="'AOZ1282CI" xr:uid="{3F6E0CD2-DB75-49F2-A69A-22FBA62FCCD3}"/>
-    <hyperlink ref="H28" r:id="rId57" tooltip="Supplier" display="'785-1613-1-ND" xr:uid="{FCB1D0F2-2759-41E6-BFF4-05B640EE4293}"/>
-    <hyperlink ref="E29" r:id="rId58" tooltip="Component" display="'Alpha &amp; Omega Semiconductor" xr:uid="{26DBEE2C-B1F8-4B2F-B22B-F99056A64074}"/>
-    <hyperlink ref="F29" r:id="rId59" tooltip="Manufacturer" display="'AOZ1284PI" xr:uid="{6AFD2339-F5BB-491F-8116-6820B9581E42}"/>
-    <hyperlink ref="H29" r:id="rId60" tooltip="Supplier" display="'785-1689-1-ND" xr:uid="{37A96A7B-64E3-4FB7-948B-07BD0B26B9B7}"/>
-    <hyperlink ref="E30" r:id="rId61" tooltip="Component" display="'Vishay Lite-On" xr:uid="{92794E04-2CED-46A2-BF83-3F89654C3D05}"/>
-    <hyperlink ref="F30" r:id="rId62" tooltip="Manufacturer" display="'LTST-C190KGKT" xr:uid="{D424A284-5963-4EC3-8ED1-254B86DA8AC4}"/>
-    <hyperlink ref="H30" r:id="rId63" tooltip="Supplier" display="'160-1435-2-ND" xr:uid="{DD55925E-3E4F-4676-927C-B8FCA1BB419F}"/>
-    <hyperlink ref="E31" r:id="rId64" tooltip="Component" display="'Vishay Lite-On" xr:uid="{95E15A37-7293-4A40-8F51-A62AC0F65C37}"/>
-    <hyperlink ref="F31" r:id="rId65" tooltip="Manufacturer" display="'LTST-C190KSKT" xr:uid="{F9C07C3F-EE61-46A7-8755-0D1119C762EE}"/>
-    <hyperlink ref="H31" r:id="rId66" tooltip="Supplier" display="'160-1437-1-ND" xr:uid="{712B5798-B365-4D63-9D82-EE6F17E5C02B}"/>
-    <hyperlink ref="E32" r:id="rId67" tooltip="Component" display="'Nexperia" xr:uid="{0F944CFB-91C6-4D06-94A1-6239F1268671}"/>
-    <hyperlink ref="F32" r:id="rId68" tooltip="Manufacturer" display="'BUK9Y21-40E,115" xr:uid="{FF5AEDA9-8DB6-429C-9740-12A88006ACFC}"/>
-    <hyperlink ref="H32" r:id="rId69" tooltip="Supplier" display="'1727-1123-1-ND" xr:uid="{31652CFE-6414-428A-9BA9-65C260FB9F03}"/>
-    <hyperlink ref="E33" r:id="rId70" tooltip="Component" display="'Nexperia" xr:uid="{C72DE173-68DD-48EC-A671-8681CDD71740}"/>
-    <hyperlink ref="F33" r:id="rId71" tooltip="Manufacturer" display="'PSMN1R8-40YLC,115" xr:uid="{8F3AF91B-1911-4604-9789-78D4CC089846}"/>
-    <hyperlink ref="H33" r:id="rId72" tooltip="Supplier" display="'1727-1052-1-ND" xr:uid="{91E17345-49F1-4AFF-9892-889D3037B4B5}"/>
-    <hyperlink ref="E34" r:id="rId73" tooltip="Component" display="'Bel" xr:uid="{9CAFBDF4-7192-4807-BBB3-9FD6EA8D3023}"/>
-    <hyperlink ref="F34" r:id="rId74" tooltip="Manufacturer" display="'0ZCM0020FF2G" xr:uid="{35C87402-F7F3-4D94-9CFA-24F2B3423261}"/>
-    <hyperlink ref="H34" r:id="rId75" tooltip="Supplier" display="'507-1821-1-ND" xr:uid="{2EDFAE02-BE4A-43DB-B4BC-6E46E3393884}"/>
-    <hyperlink ref="E35" r:id="rId76" tooltip="Component" display="'Yageo" xr:uid="{C283909A-3765-4AA7-BF17-E42C2274A59C}"/>
-    <hyperlink ref="F35" r:id="rId77" tooltip="Manufacturer" display="'RC0603FR-071KL" xr:uid="{F2A7384D-34B7-4E3A-B2C4-8135731A0F65}"/>
-    <hyperlink ref="H35" r:id="rId78" tooltip="Supplier" display="'311-1.00KHRCT-ND" xr:uid="{105845A9-9F28-40AC-83F6-C40080EF7432}"/>
-    <hyperlink ref="E36" r:id="rId79" tooltip="Component" display="'Yageo" xr:uid="{DFF08991-C313-4867-B09E-7B895C3CD1A6}"/>
-    <hyperlink ref="F36" r:id="rId80" tooltip="Manufacturer" display="'RC0603FR-071ML" xr:uid="{6FBD9E7E-5066-489A-9F61-3C567E276AA3}"/>
-    <hyperlink ref="H36" r:id="rId81" tooltip="Supplier" display="'311-1.00MHRDKR-ND" xr:uid="{EBBEC014-E7E5-40AF-A87A-DE90E972625B}"/>
-    <hyperlink ref="E37" r:id="rId82" tooltip="Component" display="'Yageo" xr:uid="{43D691ED-FC4A-40C4-849F-B425724B1715}"/>
-    <hyperlink ref="F37" r:id="rId83" tooltip="Manufacturer" display="'RC0603FR-074K7L" xr:uid="{B6E3F244-E513-447D-9AA2-DB11A4B04BEC}"/>
-    <hyperlink ref="H37" r:id="rId84" tooltip="Supplier" display="'311-4.70KHRCT-ND" xr:uid="{33A8EDA0-7D06-44A1-96BF-0714738C616D}"/>
-    <hyperlink ref="E38" r:id="rId85" tooltip="Component" display="'Yageo Phycomp" xr:uid="{3B333E4D-3AD0-4443-98BB-D8AACE657E97}"/>
-    <hyperlink ref="F38" r:id="rId86" tooltip="Manufacturer" display="'RC0603FR-0710KL" xr:uid="{0D798429-A27F-49D7-8225-1AE1A199C1D1}"/>
-    <hyperlink ref="H38" r:id="rId87" tooltip="Supplier" display="'311-10.0KHRCT-ND" xr:uid="{67D1A6AB-A003-40EE-8AEC-44ADF9AE9615}"/>
-    <hyperlink ref="E39" r:id="rId88" tooltip="Component" display="'Yageo" xr:uid="{73D855FD-BF43-4ED1-A9E8-FCA79D1D9D8C}"/>
-    <hyperlink ref="F39" r:id="rId89" tooltip="Manufacturer" display="'RC0603FR-0722RL" xr:uid="{27AC0026-2DF9-4B7F-9F72-F22B5505B8A4}"/>
-    <hyperlink ref="H39" r:id="rId90" tooltip="Supplier" display="'311-22.0HRCT-ND" xr:uid="{5B816FAE-B377-457C-B669-69680E61C2ED}"/>
-    <hyperlink ref="E40" r:id="rId91" tooltip="Component" display="'Yageo" xr:uid="{F4118BBC-E295-4CDA-B3F0-B6E0D7B992EF}"/>
-    <hyperlink ref="F40" r:id="rId92" tooltip="Manufacturer" display="'RC0603FR-0754K9L" xr:uid="{F99391B8-CF6F-42C0-BDF7-D19865235007}"/>
-    <hyperlink ref="H40" r:id="rId93" tooltip="Supplier" display="'311-54.9KHRCT-ND" xr:uid="{7F367C9B-F891-4E59-9E09-7D32B7FC82A9}"/>
-    <hyperlink ref="E41" r:id="rId94" tooltip="Component" display="'Yageo" xr:uid="{F7761A67-9BA7-437A-8B63-72E47A5275F5}"/>
-    <hyperlink ref="F41" r:id="rId95" tooltip="Manufacturer" display="'RC0603FR-07100KL" xr:uid="{6F80819B-900C-402A-AC85-E8BA139C5955}"/>
-    <hyperlink ref="H41" r:id="rId96" tooltip="Supplier" display="'311-100KHRCT-ND" xr:uid="{36D450EA-58F0-41D0-96FD-09E37FC6E33D}"/>
-    <hyperlink ref="E42" r:id="rId97" tooltip="Component" display="'Yageo" xr:uid="{D888AC08-4265-4C81-8623-6DE0772CABED}"/>
-    <hyperlink ref="F42" r:id="rId98" tooltip="Manufacturer" display="'RC0603FR-07140KL" xr:uid="{3A61D007-32C5-46F2-AF22-0C7162827294}"/>
-    <hyperlink ref="H42" r:id="rId99" tooltip="Supplier" display="'311-140KHRCT-ND" xr:uid="{86967567-5C70-4DC4-8169-09EEB385785A}"/>
-    <hyperlink ref="E43" r:id="rId100" tooltip="Component" display="'Phoenix Contact" xr:uid="{55E94060-9976-42E4-BBED-17FC683D4771}"/>
-    <hyperlink ref="F43" r:id="rId101" tooltip="Manufacturer" display="'1935776" xr:uid="{DD2DFDF2-7049-4A87-8843-E8DF2214E6E4}"/>
-    <hyperlink ref="H43" r:id="rId102" tooltip="Supplier" display="'277-6405-ND" xr:uid="{483CAE57-6918-4CD5-A865-F9D3C1AE67A8}"/>
-    <hyperlink ref="E44" r:id="rId103" tooltip="Component" display="'Wurth Electronics" xr:uid="{9CEED206-CE7E-4875-8891-2AF5CA942DFA}"/>
-    <hyperlink ref="F44" r:id="rId104" tooltip="Manufacturer" display="'416131160803" xr:uid="{4F2E35BF-03AE-412E-AAA2-3A3FDFBBA167}"/>
-    <hyperlink ref="H44" r:id="rId105" tooltip="Supplier" display="'732-3853-1-ND" xr:uid="{B62C968E-48B4-4C28-AD84-47E8A8D8C97A}"/>
-    <hyperlink ref="E45" r:id="rId106" tooltip="Component" display="'APEM" xr:uid="{4BD5395F-8BAC-4CF7-9F00-6A42C08C0F76}"/>
-    <hyperlink ref="F45" r:id="rId107" tooltip="Manufacturer" display="'MJTP1106SATR" xr:uid="{A67FD5D6-4B39-4D37-90B6-9EDCE9B98AF5}"/>
-    <hyperlink ref="H45" r:id="rId108" tooltip="Supplier" display="'679-2396-1-ND" xr:uid="{B752F897-6BC7-4838-B3F1-F5C8A9C02CD6}"/>
-    <hyperlink ref="E46" r:id="rId109" tooltip="Component" display="'Phoenix Contact" xr:uid="{BDBD4A50-6298-4B4B-96D5-85E7C666013A}"/>
-    <hyperlink ref="F46" r:id="rId110" tooltip="Manufacturer" display="'MKDS1/2-3,5" xr:uid="{7509203E-4529-449B-A9A3-A1FA617CA7BC}"/>
-    <hyperlink ref="H46" r:id="rId111" tooltip="Supplier" display="'277-5719-ND" xr:uid="{BED0BC76-8DBD-43F3-A10E-B8C06164B6BE}"/>
-    <hyperlink ref="E47" r:id="rId112" tooltip="Component" display="'Phoenix Contact" xr:uid="{E20229B9-3DA9-4F2E-97BE-34FEF188DEC0}"/>
-    <hyperlink ref="F47" r:id="rId113" tooltip="Manufacturer" display="'1935776" xr:uid="{8E6B2E95-913A-426B-AEFA-5FD7B7021376}"/>
-    <hyperlink ref="H47" r:id="rId114" tooltip="Supplier" display="'277-6405-ND" xr:uid="{8E525B14-638A-4502-8A7D-7902245C0B68}"/>
-    <hyperlink ref="E48" r:id="rId115" tooltip="Component" display="'Phoenix Contact" xr:uid="{54BE62A7-06C7-4440-A7C8-B7D812107755}"/>
-    <hyperlink ref="F48" r:id="rId116" tooltip="Manufacturer" display="'MKDS1/4-3,5" xr:uid="{510BAE87-A6E6-4966-AEDF-89D1441584A2}"/>
-    <hyperlink ref="H48" r:id="rId117" tooltip="Supplier" display="'277-5744-ND" xr:uid="{97129B05-FAF6-49EB-BE21-CE4E213CED30}"/>
-    <hyperlink ref="E49" r:id="rId118" tooltip="Component" display="'STMicroelectronics" xr:uid="{5F789EEA-5EE8-4A1D-B5E8-983DBBE92A20}"/>
-    <hyperlink ref="F49" r:id="rId119" tooltip="Manufacturer" display="'USBLC6-4SC6" xr:uid="{6BCAFF01-3E46-4E13-B828-EFDE8EF0CCE6}"/>
-    <hyperlink ref="H49" r:id="rId120" tooltip="Supplier" display="'497-4492-1-ND" xr:uid="{FA73E27D-9674-4D69-9495-09DBDCAAA9A3}"/>
+    <hyperlink ref="E2" r:id="rId1" tooltip="Component" display="'Sullins" xr:uid="{18FFE07C-B9D6-4B6A-9734-A9069DC905FB}"/>
+    <hyperlink ref="F2" r:id="rId2" tooltip="Manufacturer" display="'QPC02SXGN-RC" xr:uid="{EE0B2014-7C08-4DC1-AAF3-EBC5F47E7E94}"/>
+    <hyperlink ref="H2" r:id="rId3" tooltip="Supplier" display="'S9337-ND" xr:uid="{7B98D141-3763-4804-9692-9B108BEC5204}"/>
+    <hyperlink ref="E3" r:id="rId4" tooltip="Component" display="'Panasonic" xr:uid="{0AE861E4-17DA-449F-BDDC-0F25F7EEBF5A}"/>
+    <hyperlink ref="F3" r:id="rId5" tooltip="Manufacturer" display="'EEEFT1V101AP" xr:uid="{A7D344B5-74FB-47C7-A563-2D8350F7A90B}"/>
+    <hyperlink ref="H3" r:id="rId6" tooltip="Supplier" display="'PCE5016CT-ND" xr:uid="{7FB3CC7E-FB9C-4241-9866-E7E0F2AC6C6E}"/>
+    <hyperlink ref="E4" r:id="rId7" tooltip="Component" display="'Yageo" xr:uid="{B3C8EE4F-DE55-48BC-8CC3-FE0439D9AFB9}"/>
+    <hyperlink ref="F4" r:id="rId8" tooltip="Manufacturer" display="'CC0603KRX7R9BB104" xr:uid="{5D795B99-B5AD-482C-A5B9-FE03A6E0E22D}"/>
+    <hyperlink ref="H4" r:id="rId9" tooltip="Supplier" display="'311-1344-1-ND" xr:uid="{83CC2747-B1A8-4655-B140-12A4C843044C}"/>
+    <hyperlink ref="E5" r:id="rId10" tooltip="Component" display="'Taiyo Yuden" xr:uid="{8DDE42DC-F9B8-43B0-A536-5370D6E26F24}"/>
+    <hyperlink ref="F5" r:id="rId11" tooltip="Manufacturer" display="'EMK107B7105KA-T" xr:uid="{EB4329E6-37EF-4D80-94A0-08E4C8036849}"/>
+    <hyperlink ref="H5" r:id="rId12" tooltip="Supplier" display="'587-1241-1-ND" xr:uid="{A230B8EE-B33D-4EEE-9FD6-91BEF1195130}"/>
+    <hyperlink ref="E6" r:id="rId13" tooltip="Component" display="'TDK" xr:uid="{4AE40066-9B9C-49F5-801E-7C72D31EC668}"/>
+    <hyperlink ref="F6" r:id="rId14" tooltip="Manufacturer" display="'C2012X7R1A475K085AC" xr:uid="{AE2A619B-4CD7-4FE5-BD4A-535B6525EB3F}"/>
+    <hyperlink ref="H6" r:id="rId15" tooltip="Supplier" display="'445-14527-1-ND" xr:uid="{E8DD9280-DF20-4A73-BB21-60708746463B}"/>
+    <hyperlink ref="E7" r:id="rId16" tooltip="Component" display="'KEMET" xr:uid="{C0E39A4B-9BE8-46C6-A072-116D86C2AC71}"/>
+    <hyperlink ref="F7" r:id="rId17" tooltip="Manufacturer" display="'C1210C475K5RACTU" xr:uid="{E91002BD-CD2E-441F-84F2-63EE7C3DCB2B}"/>
+    <hyperlink ref="H7" r:id="rId18" tooltip="Supplier" display="'399-6785-1-ND" xr:uid="{BF7EA0E6-8C12-49CC-BFB1-FA1706DFF7E6}"/>
+    <hyperlink ref="E8" r:id="rId19" tooltip="Component" display="'Kyocera AVX" xr:uid="{F3229103-2999-4BC2-BC46-43B47C87488D}"/>
+    <hyperlink ref="F8" r:id="rId20" tooltip="Manufacturer" display="'06035C220JAT2A" xr:uid="{8E1D1029-5D55-4291-A342-1A273345895F}"/>
+    <hyperlink ref="H8" r:id="rId21" tooltip="Supplier" display="'478-6204-1-ND" xr:uid="{68F635F1-43C4-42D3-ADE5-1112F06C3EEB}"/>
+    <hyperlink ref="E9" r:id="rId22" tooltip="Component" display="'Molex" xr:uid="{D4EEA83F-2E5B-4C84-9453-4260B9D1A37A}"/>
+    <hyperlink ref="F9" r:id="rId23" tooltip="Manufacturer" display="'105017-0001" xr:uid="{A87ACEDF-4AC8-4F84-927D-51C7593EDF35}"/>
+    <hyperlink ref="H9" r:id="rId24" tooltip="Supplier" display="'WM1399CT-ND" xr:uid="{03EFD7C6-11BD-47A5-A136-C42566C4D48F}"/>
+    <hyperlink ref="E10" r:id="rId25" tooltip="Component" display="'Epson" xr:uid="{CF188930-39CA-4FE7-ABF4-79BE5D351389}"/>
+    <hyperlink ref="F10" r:id="rId26" tooltip="Manufacturer" display="'FA-23816.0000MBC3" xr:uid="{600102B5-8561-4673-9F0E-DF27E9DB6C96}"/>
+    <hyperlink ref="H10" r:id="rId27" tooltip="Supplier" display="'SER3686CT-ND" xr:uid="{D0B776FB-153F-4C25-AAB1-C7AD189BDC8C}"/>
+    <hyperlink ref="E11" r:id="rId28" tooltip="Component" display="'MCC" xr:uid="{CF07150C-7C2C-4293-BB6D-7C600D9F2F8C}"/>
+    <hyperlink ref="F11" r:id="rId29" tooltip="Manufacturer" display="'1N4148WX-TP" xr:uid="{EA387FDA-61FC-4E5D-9EAC-5EF07BF49F18}"/>
+    <hyperlink ref="H11" r:id="rId30" tooltip="Supplier" display="'1N4148WXTPMSCT-ND" xr:uid="{CC8131CC-B24D-4D6A-BFDC-C9DEE81047BA}"/>
+    <hyperlink ref="E12" r:id="rId31" tooltip="Component" display="'Diodes" xr:uid="{51E6A4A0-41B1-4E59-B697-F97EE92B663D}"/>
+    <hyperlink ref="F12" r:id="rId32" tooltip="Manufacturer" display="'S2BA-13-F" xr:uid="{E5D1EDD0-9DA5-43E4-A281-61DC2DA09215}"/>
+    <hyperlink ref="H12" r:id="rId33" tooltip="Supplier" display="'S2BA-FDICT-ND" xr:uid="{A509BDC4-4399-4AC3-A311-48D027D2FDC6}"/>
+    <hyperlink ref="E13" r:id="rId34" tooltip="Component" display="'ON Semiconductor / Fairchild" xr:uid="{1132AEFC-EC2E-4A94-8B4F-75B20695EA41}"/>
+    <hyperlink ref="F13" r:id="rId35" tooltip="Manufacturer" display="'SS24FL" xr:uid="{A436CABE-5064-43A0-AB87-688B0B881FBC}"/>
+    <hyperlink ref="H13" r:id="rId36" tooltip="Supplier" display="'SS24FLCT-ND" xr:uid="{36964338-A09C-44BA-B63B-CA6C1F13614E}"/>
+    <hyperlink ref="E14" r:id="rId37" tooltip="Component" display="'General Instruments" xr:uid="{03EB735C-A646-488D-A1E1-A2CEE9616D5A}"/>
+    <hyperlink ref="F14" r:id="rId38" tooltip="Manufacturer" display="'SSB44-E3/52T" xr:uid="{C28C8AB6-9553-4F55-9C68-95D60C467C58}"/>
+    <hyperlink ref="H14" r:id="rId39" tooltip="Supplier" display="'SSB44-E3/52TGICT-ND" xr:uid="{46A32CB5-DAEB-4CB6-AD51-5F193A249DBB}"/>
+    <hyperlink ref="E15" r:id="rId40" tooltip="Component" display="'Murata" xr:uid="{39AB10D9-5921-4DC9-A812-F5604178B0C4}"/>
+    <hyperlink ref="F15" r:id="rId41" tooltip="Manufacturer" display="'BLM21PG221SN1D" xr:uid="{58D602EC-9DD9-468A-AFB4-A0AA486DA142}"/>
+    <hyperlink ref="H15" r:id="rId42" tooltip="Supplier" display="'490-1054-1-ND" xr:uid="{62E8DF54-324F-431A-9DF8-AA9CC10B6CA3}"/>
+    <hyperlink ref="E16" r:id="rId43" tooltip="Component" display="'Bourns" xr:uid="{973710B0-073E-43E6-9110-A1A8125A9CB6}"/>
+    <hyperlink ref="F16" r:id="rId44" tooltip="Manufacturer" display="'SRN6045TA-4R7M" xr:uid="{AC2EBE50-B138-4E87-B5D9-8799E67612F1}"/>
+    <hyperlink ref="H16" r:id="rId45" tooltip="Supplier" display="'SRN6045TA-4R7MCT-ND" xr:uid="{558932F0-8975-4F28-9C42-40A3E4D39E22}"/>
+    <hyperlink ref="E17" r:id="rId46" tooltip="Component" display="'Bourns" xr:uid="{73563059-8E9E-4215-A45B-A2CBF1097B1D}"/>
+    <hyperlink ref="F17" r:id="rId47" tooltip="Manufacturer" display="'SRN6045TA-330M" xr:uid="{467E5FA0-DEA9-4A3D-9B24-13565C1598B0}"/>
+    <hyperlink ref="H17" r:id="rId48" tooltip="Supplier" display="'SRN6045TA-330MCT-ND" xr:uid="{CB22681E-7653-4820-9553-3CAF97895E23}"/>
+    <hyperlink ref="E18" r:id="rId49" tooltip="Component" display="'Memory Protection Devices" xr:uid="{CF94C808-FAC5-4D1F-8E50-EDD5BC35F8A5}"/>
+    <hyperlink ref="F18" r:id="rId50" tooltip="Manufacturer" display="'BK-6013" xr:uid="{25387055-DB07-4B11-A2AD-AFE393873C7E}"/>
+    <hyperlink ref="H18" r:id="rId51" tooltip="Supplier" display="'BK-6013-ND" xr:uid="{26AC93FE-B107-4927-97C1-DD54E3D648B7}"/>
+    <hyperlink ref="E19" tooltip="Component" display="'Generic Header" xr:uid="{17981523-1AAB-41E4-8FFF-E371BCD3B8C0}"/>
+    <hyperlink ref="F19" tooltip="Manufacturer" display="'" xr:uid="{DF814CA7-B673-4654-8D91-29971A0DDBEA}"/>
+    <hyperlink ref="H19" tooltip="Supplier" display="'" xr:uid="{A0B866E5-89D8-48CC-A44D-4C63F4FEB815}"/>
+    <hyperlink ref="E20" tooltip="Component" display="'Generic Header" xr:uid="{0147D1A4-BC0D-48DA-A186-C8A9D0179765}"/>
+    <hyperlink ref="F20" tooltip="Manufacturer" display="'" xr:uid="{9617B630-C11C-47ED-A821-A488CAF1D6EE}"/>
+    <hyperlink ref="H20" tooltip="Supplier" display="'" xr:uid="{686298E3-C983-4033-A2C5-9B0DC0383B2F}"/>
+    <hyperlink ref="E21" tooltip="Component" display="'Generic Header" xr:uid="{74E654E8-CCBE-409B-8785-A668B173CBB6}"/>
+    <hyperlink ref="F21" tooltip="Manufacturer" display="'" xr:uid="{8E86070A-8272-4628-AFC1-463F125554A7}"/>
+    <hyperlink ref="H21" tooltip="Supplier" display="'" xr:uid="{D625EA45-8CA4-468D-8BDA-4F556B2BB602}"/>
+    <hyperlink ref="E22" tooltip="Component" display="'Generic Header" xr:uid="{651F0FF8-BF33-4BC6-A987-C97D90248F13}"/>
+    <hyperlink ref="F22" tooltip="Manufacturer" display="'" xr:uid="{0552AE54-19FE-40EB-9E6F-78F2E554CE60}"/>
+    <hyperlink ref="H22" tooltip="Supplier" display="'" xr:uid="{73BD28F3-56CF-4BC7-A9BB-8A29DB387BC7}"/>
+    <hyperlink ref="E23" tooltip="Component" display="'Generic Header" xr:uid="{B3FDF792-9259-4982-8069-0A842B39EABA}"/>
+    <hyperlink ref="F23" tooltip="Manufacturer" display="'" xr:uid="{76A80EDB-7768-40FC-867E-7C3609EE4B5D}"/>
+    <hyperlink ref="H23" tooltip="Supplier" display="'" xr:uid="{CD2059CF-9D99-457C-BAF1-C05ACACFA4DC}"/>
+    <hyperlink ref="E24" tooltip="Component" display="'Generic Header" xr:uid="{437DA3E8-DCFD-4D43-BC38-D612278C4B6C}"/>
+    <hyperlink ref="F24" tooltip="Manufacturer" display="'" xr:uid="{BDF11DF0-270F-4774-B723-69B5D32D4A11}"/>
+    <hyperlink ref="H24" tooltip="Supplier" display="'" xr:uid="{28B3DF9F-F730-445A-8DAE-48940E867683}"/>
+    <hyperlink ref="E25" tooltip="Component" display="'Generic Header" xr:uid="{65C6AC99-5CF8-4408-9B76-BDB5BC8B9556}"/>
+    <hyperlink ref="F25" tooltip="Manufacturer" display="'" xr:uid="{C7370E5A-7EE5-4C75-B3B1-5FD4343FDA92}"/>
+    <hyperlink ref="H25" tooltip="Supplier" display="'" xr:uid="{8B8E38EA-5711-4AC7-B325-6F190DF2AEB8}"/>
+    <hyperlink ref="E26" tooltip="Component" display="'Generic Header" xr:uid="{8C0E7341-A0F3-4FA7-89F9-46DC5AC28178}"/>
+    <hyperlink ref="F26" tooltip="Manufacturer" display="'" xr:uid="{47CED069-12FD-457D-9EE7-55BCB610C355}"/>
+    <hyperlink ref="H26" tooltip="Supplier" display="'" xr:uid="{29853A20-91F7-4608-8659-8B51823DADAB}"/>
+    <hyperlink ref="E27" r:id="rId52" tooltip="Component" display="'Microchip" xr:uid="{D0CA0E5C-C7C4-41A2-8939-8C6E6972A3D4}"/>
+    <hyperlink ref="F27" r:id="rId53" tooltip="Manufacturer" display="'ATMEGA16U2-MU" xr:uid="{7B4DE4F3-6BCE-4A19-BF7B-EE9621FC6A06}"/>
+    <hyperlink ref="H27" r:id="rId54" tooltip="Supplier" display="'ATMEGA16U2-MU-ND" xr:uid="{658E5DF8-79DC-4BC8-90D2-61F9982FBF29}"/>
+    <hyperlink ref="E28" r:id="rId55" tooltip="Component" display="'Microchip / Atmel" xr:uid="{8832A901-2E87-4825-9159-9BFB4D42D0B3}"/>
+    <hyperlink ref="F28" r:id="rId56" tooltip="Manufacturer" display="'ATMEGA2560-16AU" xr:uid="{198EE85A-7696-45F2-82D8-832AA4C096F8}"/>
+    <hyperlink ref="H28" r:id="rId57" tooltip="Supplier" display="'ATMEGA2560-16AU-ND" xr:uid="{51CA8A4E-C153-4DD3-AD06-09615A52FA58}"/>
+    <hyperlink ref="E29" r:id="rId58" tooltip="Component" display="'Alpha &amp; Omega Semiconductor" xr:uid="{9386B762-A9E8-45F6-9DF5-29E51663B8F8}"/>
+    <hyperlink ref="F29" r:id="rId59" tooltip="Manufacturer" display="'AOZ1282CI" xr:uid="{ACA6B6E8-C00D-4019-992D-A7D09409D165}"/>
+    <hyperlink ref="H29" r:id="rId60" tooltip="Supplier" display="'785-1613-1-ND" xr:uid="{E4FB99C1-90D1-491E-9090-69A3FD479155}"/>
+    <hyperlink ref="E30" r:id="rId61" tooltip="Component" display="'Alpha &amp; Omega Semiconductor" xr:uid="{6C8C9BFB-E9D4-40B3-850C-3B1828B8BC44}"/>
+    <hyperlink ref="F30" r:id="rId62" tooltip="Manufacturer" display="'AOZ1284PI" xr:uid="{7DF4A19A-7745-45D3-8141-E0D11AD7564E}"/>
+    <hyperlink ref="H30" r:id="rId63" tooltip="Supplier" display="'785-1689-1-ND" xr:uid="{1CCA2ABF-6CBD-449C-814F-9646BB01B852}"/>
+    <hyperlink ref="E31" r:id="rId64" tooltip="Component" display="'Vishay Lite-On" xr:uid="{6AA8530B-B4C6-4151-925F-4A2E8D07DB82}"/>
+    <hyperlink ref="F31" r:id="rId65" tooltip="Manufacturer" display="'LTST-C190KGKT" xr:uid="{ED9556D0-7F9F-4002-B53D-C14E08EB6B4D}"/>
+    <hyperlink ref="H31" r:id="rId66" tooltip="Supplier" display="'160-1435-2-ND" xr:uid="{1E34BE3D-5018-4DB3-B177-8D0AA8ABFFEB}"/>
+    <hyperlink ref="E32" r:id="rId67" tooltip="Component" display="'Vishay Lite-On" xr:uid="{3F92821E-E531-42A9-8E2F-996E7C67D9FE}"/>
+    <hyperlink ref="F32" r:id="rId68" tooltip="Manufacturer" display="'LTST-C190KSKT" xr:uid="{44AC24A8-C3C2-4284-948F-3ACE65253177}"/>
+    <hyperlink ref="H32" r:id="rId69" tooltip="Supplier" display="'160-1437-1-ND" xr:uid="{1F39453E-CAF5-4E22-8115-E5588A6D1E9F}"/>
+    <hyperlink ref="E33" r:id="rId70" tooltip="Component" display="'Nexperia" xr:uid="{CD214499-CCF8-454D-B1C8-180D0E9BFBD1}"/>
+    <hyperlink ref="F33" r:id="rId71" tooltip="Manufacturer" display="'BUK9Y21-40E,115" xr:uid="{A6EAEBA3-20E7-4CAD-A674-3B21FBDB7D77}"/>
+    <hyperlink ref="H33" r:id="rId72" tooltip="Supplier" display="'1727-1123-1-ND" xr:uid="{541E6359-FE0D-4082-9A91-CF792109EA4E}"/>
+    <hyperlink ref="E34" r:id="rId73" tooltip="Component" display="'Nexperia" xr:uid="{FCAA6503-7162-4D04-A7DB-B9DA6FCC4712}"/>
+    <hyperlink ref="F34" r:id="rId74" tooltip="Manufacturer" display="'PSMN1R8-40YLC,115" xr:uid="{53C7FE7D-7D10-4BE7-B068-E2B73F494C45}"/>
+    <hyperlink ref="H34" r:id="rId75" tooltip="Supplier" display="'1727-1052-1-ND" xr:uid="{7781CD66-3E96-432F-8E17-06F38D98380B}"/>
+    <hyperlink ref="E35" r:id="rId76" tooltip="Component" display="'Bel" xr:uid="{A529F792-C65B-4CEC-B3AE-21958BBFA38C}"/>
+    <hyperlink ref="F35" r:id="rId77" tooltip="Manufacturer" display="'0ZCM0020FF2G" xr:uid="{A015EF64-DBC5-47F1-A887-430C7DE765F1}"/>
+    <hyperlink ref="H35" r:id="rId78" tooltip="Supplier" display="'507-1821-1-ND" xr:uid="{8F15F700-2C53-42C8-96C8-D9900EF9FA0B}"/>
+    <hyperlink ref="E36" r:id="rId79" tooltip="Component" display="'Yageo" xr:uid="{DBE8B3BC-D024-47EC-9B26-28C5B489E79C}"/>
+    <hyperlink ref="F36" r:id="rId80" tooltip="Manufacturer" display="'RC0603FR-071KL" xr:uid="{5B657405-52CB-472C-A3B1-500B622EF0AF}"/>
+    <hyperlink ref="H36" r:id="rId81" tooltip="Supplier" display="'311-1.00KHRCT-ND" xr:uid="{B51AA361-47C4-4467-957B-7ED0506042A1}"/>
+    <hyperlink ref="E37" r:id="rId82" tooltip="Component" display="'Yageo" xr:uid="{42C95FA4-3040-495D-9E40-D1BF593E2C19}"/>
+    <hyperlink ref="F37" r:id="rId83" tooltip="Manufacturer" display="'RC0603FR-071ML" xr:uid="{A3D9121D-8D97-40DF-845F-280229F492A8}"/>
+    <hyperlink ref="H37" r:id="rId84" tooltip="Supplier" display="'311-1.00MHRDKR-ND" xr:uid="{DEB0C63B-8D40-473E-A5C1-5B9E04E92E41}"/>
+    <hyperlink ref="E38" r:id="rId85" tooltip="Component" display="'Yageo" xr:uid="{A8CCBA26-7C17-45E8-B9FF-E6DC24226774}"/>
+    <hyperlink ref="F38" r:id="rId86" tooltip="Manufacturer" display="'RC0603FR-074K7L" xr:uid="{7A04B63B-C092-4063-A382-F46A49DC1EC0}"/>
+    <hyperlink ref="H38" r:id="rId87" tooltip="Supplier" display="'311-4.70KHRCT-ND" xr:uid="{ED3B3D1B-05B2-42E5-B405-E678AF5D1F89}"/>
+    <hyperlink ref="E39" r:id="rId88" tooltip="Component" display="'Yageo Phycomp" xr:uid="{C170B6C2-C908-4D18-B882-805BF091394A}"/>
+    <hyperlink ref="F39" r:id="rId89" tooltip="Manufacturer" display="'RC0603FR-0710KL" xr:uid="{77B54149-1DD0-4A2A-9EC3-179464E0D1A5}"/>
+    <hyperlink ref="H39" r:id="rId90" tooltip="Supplier" display="'311-10.0KHRCT-ND" xr:uid="{42A39318-97FF-43D5-8DE2-6D6EBAFA1030}"/>
+    <hyperlink ref="E40" r:id="rId91" tooltip="Component" display="'Yageo" xr:uid="{4BC6B98F-2A2C-4187-9401-A927410A92B0}"/>
+    <hyperlink ref="F40" r:id="rId92" tooltip="Manufacturer" display="'RC0603FR-0722RL" xr:uid="{7A8C26E9-8B69-4E0A-B726-310C63310E45}"/>
+    <hyperlink ref="H40" r:id="rId93" tooltip="Supplier" display="'311-22.0HRCT-ND" xr:uid="{7142CFE1-C29D-490C-AB33-D6A1EA7DAC23}"/>
+    <hyperlink ref="E41" r:id="rId94" tooltip="Component" display="'Yageo" xr:uid="{1C8EE593-F1D5-4DBC-893B-6FE18DE55873}"/>
+    <hyperlink ref="F41" r:id="rId95" tooltip="Manufacturer" display="'RC0603FR-0754K9L" xr:uid="{A9563202-E7A3-4487-9BDD-7EDA0FC00F62}"/>
+    <hyperlink ref="H41" r:id="rId96" tooltip="Supplier" display="'311-54.9KHRCT-ND" xr:uid="{5885893E-A5A7-4A91-9627-EEEDBD6AB421}"/>
+    <hyperlink ref="E42" r:id="rId97" tooltip="Component" display="'Yageo" xr:uid="{BCD7CE7F-E90B-46C5-8A50-26CBC581EA92}"/>
+    <hyperlink ref="F42" r:id="rId98" tooltip="Manufacturer" display="'RC0603FR-07100KL" xr:uid="{042C247A-8F67-45E8-8FD4-7B34B26C5BD4}"/>
+    <hyperlink ref="H42" r:id="rId99" tooltip="Supplier" display="'311-100KHRCT-ND" xr:uid="{60A590F5-56E5-46BB-8E4C-9685D7D9F731}"/>
+    <hyperlink ref="E43" r:id="rId100" tooltip="Component" display="'Yageo" xr:uid="{82B6DFAC-D5E9-4791-B4B3-60E3600097B2}"/>
+    <hyperlink ref="F43" r:id="rId101" tooltip="Manufacturer" display="'RC0603FR-07140KL" xr:uid="{66B160E5-8231-4954-94B0-4100EA04B270}"/>
+    <hyperlink ref="H43" r:id="rId102" tooltip="Supplier" display="'311-140KHRCT-ND" xr:uid="{2E56ADC8-FB9B-44AE-AFFD-B5E96D2A3D78}"/>
+    <hyperlink ref="E44" r:id="rId103" tooltip="Component" display="'Phoenix Contact" xr:uid="{088E67CA-220E-4BD5-9E76-733A3E8D23A9}"/>
+    <hyperlink ref="F44" r:id="rId104" tooltip="Manufacturer" display="'1935776" xr:uid="{F695651C-14DB-4EA2-9F09-2E6E93D61B80}"/>
+    <hyperlink ref="H44" r:id="rId105" tooltip="Supplier" display="'277-6405-ND" xr:uid="{B04DC7E3-F4A7-4920-BFC7-17D36F1EB94A}"/>
+    <hyperlink ref="E45" r:id="rId106" tooltip="Component" display="'Wurth Electronics" xr:uid="{CC6DA31F-7290-4B80-9764-BC58FB1B7DCA}"/>
+    <hyperlink ref="F45" r:id="rId107" tooltip="Manufacturer" display="'416131160803" xr:uid="{FFD27985-E647-4168-B2D0-0B70A5F79680}"/>
+    <hyperlink ref="H45" r:id="rId108" tooltip="Supplier" display="'732-3853-1-ND" xr:uid="{5DF1E3B3-E753-4C3F-A835-0E640EAE7807}"/>
+    <hyperlink ref="E46" r:id="rId109" tooltip="Component" display="'APEM" xr:uid="{22FEE83A-2045-4BD7-B215-B781D11D260C}"/>
+    <hyperlink ref="F46" r:id="rId110" tooltip="Manufacturer" display="'MJTP1106SATR" xr:uid="{EADA80B8-FA87-41DC-BB69-E959AA5B0501}"/>
+    <hyperlink ref="H46" r:id="rId111" tooltip="Supplier" display="'679-2396-1-ND" xr:uid="{98E18E9B-C028-4653-B781-5AA5C3F68B66}"/>
+    <hyperlink ref="E47" r:id="rId112" tooltip="Component" display="'Phoenix Contact" xr:uid="{F50F065E-564B-4064-9EB5-B3DBBC62BE0C}"/>
+    <hyperlink ref="F47" r:id="rId113" tooltip="Manufacturer" display="'MKDS1/2-3,5" xr:uid="{A0143C42-7365-45FB-818D-2343B688B629}"/>
+    <hyperlink ref="H47" r:id="rId114" tooltip="Supplier" display="'277-5719-ND" xr:uid="{8DF0C021-49C5-4E3C-8E46-2955015D4F8C}"/>
+    <hyperlink ref="E48" r:id="rId115" tooltip="Component" display="'Phoenix Contact" xr:uid="{ED4A4352-F6E8-4B05-9947-9A7EFEA54AFD}"/>
+    <hyperlink ref="F48" r:id="rId116" tooltip="Manufacturer" display="'1935776" xr:uid="{37235D55-5EB8-4FEB-9CB3-BC40A227B48F}"/>
+    <hyperlink ref="H48" r:id="rId117" tooltip="Supplier" display="'277-6405-ND" xr:uid="{E8C8FE7F-A5BD-4D3C-B307-62BC4AEBD150}"/>
+    <hyperlink ref="E49" r:id="rId118" tooltip="Component" display="'Phoenix Contact" xr:uid="{71C3241E-BCEF-4F45-BE8A-1956001D2C20}"/>
+    <hyperlink ref="F49" r:id="rId119" tooltip="Manufacturer" display="'MKDS1/4-3,5" xr:uid="{252646B8-4648-4A50-9839-CF73079B3A17}"/>
+    <hyperlink ref="H49" r:id="rId120" tooltip="Supplier" display="'277-5744-ND" xr:uid="{46A0B8D6-B076-4370-A067-801D7E59C8D9}"/>
+    <hyperlink ref="E50" r:id="rId121" tooltip="Component" display="'STMicroelectronics" xr:uid="{7E849632-75DA-4593-9591-8782F9AAA5E0}"/>
+    <hyperlink ref="F50" r:id="rId122" tooltip="Manufacturer" display="'USBLC6-4SC6" xr:uid="{55F6D486-0982-41B4-A76F-387F13064C0A}"/>
+    <hyperlink ref="H50" r:id="rId123" tooltip="Supplier" display="'497-4492-1-ND" xr:uid="{8CD75313-3DFD-4D91-8BC3-D24DC503E9BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId121"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId124"/>
 </worksheet>
 </file>
</xml_diff>